<commit_message>
comiited - changed excel file
</commit_message>
<xml_diff>
--- a/dataread/dataExcel.xlsx
+++ b/dataread/dataExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>user4@gmail.com</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>55</t>
   </si>
 </sst>
 </file>
@@ -95,8 +86,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +392,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,10 +417,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -437,10 +428,10 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -448,10 +439,10 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -459,10 +450,10 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>